<commit_message>
second commit for sending local git to org git
</commit_message>
<xml_diff>
--- a/BULK_CONFIG_FILE/Engagement_training_config_file.xlsx
+++ b/BULK_CONFIG_FILE/Engagement_training_config_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vamsikkrishna\PycharmProjects\pythonProject1\BULK_CONFIG_FILE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDBCE3F-5178-43F3-99E2-41D2A0FC3AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFC80B0-3791-4AEF-BD8E-1A09FB997708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2362,7 +2362,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>